<commit_message>
Error fix & pick trade
</commit_message>
<xml_diff>
--- a/data/drafts.xlsx
+++ b/data/drafts.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max/Insync/rmaxsm@umich.edu/Google Drive/FF/TRUFFLE/TRUFFLEdash/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max/Insync/rmaxsm@umich.edu/Google Drive/FF/TRUFFLE/TRUFFLEdashGIT/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7998C78-E3E4-554F-92DD-71AE2FE9BD9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74AAB565-8EDB-0E44-BE0F-D662920C3223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16300" xr2:uid="{9C0D35C5-E0BD-F642-9C22-EDCA1069C401}"/>
+    <workbookView xWindow="42000" yWindow="3860" windowWidth="28800" windowHeight="16300" xr2:uid="{9C0D35C5-E0BD-F642-9C22-EDCA1069C401}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="105">
   <si>
     <t>Season</t>
   </si>
@@ -324,9 +324,6 @@
     <t>*traded from MWM</t>
   </si>
   <si>
-    <t>*traded from VD, via MCM</t>
-  </si>
-  <si>
     <t>*traded from MCM</t>
   </si>
   <si>
@@ -346,6 +343,12 @@
   </si>
   <si>
     <t>TBD</t>
+  </si>
+  <si>
+    <t>*traded from ELP</t>
+  </si>
+  <si>
+    <t>*traded from CRB, via VD &amp; MCM</t>
   </si>
 </sst>
 </file>
@@ -706,8 +709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{133FC257-8E11-CE40-AF62-7EB48A446FE4}">
   <dimension ref="A1:T109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="G98" sqref="G98"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="D84" sqref="D84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2477,11 +2480,13 @@
         <v>1</v>
       </c>
       <c r="D74" t="s">
-        <v>15</v>
-      </c>
-      <c r="E74" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>103</v>
+      </c>
       <c r="F74" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G74">
         <v>50</v>
@@ -2502,7 +2507,7 @@
       </c>
       <c r="E75" s="1"/>
       <c r="F75" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G75">
         <v>45</v>
@@ -2523,7 +2528,7 @@
       </c>
       <c r="E76" s="1"/>
       <c r="F76" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G76">
         <v>40</v>
@@ -2544,7 +2549,7 @@
       </c>
       <c r="E77" s="1"/>
       <c r="F77" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G77">
         <v>35</v>
@@ -2561,11 +2566,13 @@
         <v>5</v>
       </c>
       <c r="D78" t="s">
-        <v>12</v>
-      </c>
-      <c r="E78" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="F78" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G78">
         <v>30</v>
@@ -2586,7 +2593,7 @@
       </c>
       <c r="E79" s="1"/>
       <c r="F79" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G79">
         <v>25</v>
@@ -2607,7 +2614,7 @@
       </c>
       <c r="E80" s="1"/>
       <c r="F80" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G80">
         <v>20</v>
@@ -2627,10 +2634,10 @@
         <v>16</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F81" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G81">
         <v>15</v>
@@ -2651,7 +2658,7 @@
       </c>
       <c r="E82" s="1"/>
       <c r="F82" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G82">
         <v>15</v>
@@ -2674,7 +2681,7 @@
         <v>95</v>
       </c>
       <c r="F83" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G83">
         <v>10</v>
@@ -2691,13 +2698,13 @@
         <v>11</v>
       </c>
       <c r="D84" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="F84" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G84">
         <v>10</v>
@@ -2718,7 +2725,7 @@
       </c>
       <c r="E85" s="1"/>
       <c r="F85" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G85">
         <v>10</v>
@@ -2739,7 +2746,7 @@
       </c>
       <c r="E86" s="1"/>
       <c r="F86" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G86">
         <v>5</v>
@@ -2759,10 +2766,10 @@
         <v>5</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F87" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G87">
         <v>5</v>
@@ -2785,7 +2792,7 @@
         <v>95</v>
       </c>
       <c r="F88" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G88">
         <v>5</v>
@@ -2806,7 +2813,7 @@
       </c>
       <c r="E89" s="1"/>
       <c r="F89" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G89">
         <v>5</v>
@@ -2826,10 +2833,10 @@
         <v>12</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F90" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G90">
         <v>5</v>
@@ -2850,7 +2857,7 @@
       </c>
       <c r="E91" s="1"/>
       <c r="F91" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G91">
         <v>5</v>
@@ -2871,7 +2878,7 @@
       </c>
       <c r="E92" s="1"/>
       <c r="F92" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G92">
         <v>5</v>
@@ -2891,10 +2898,10 @@
         <v>9</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F93" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G93">
         <v>5</v>
@@ -2914,10 +2921,10 @@
         <v>9</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F94" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G94">
         <v>5</v>
@@ -2938,7 +2945,7 @@
       </c>
       <c r="E95" s="1"/>
       <c r="F95" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G95">
         <v>5</v>
@@ -2959,7 +2966,7 @@
       </c>
       <c r="E96" s="1"/>
       <c r="F96" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G96">
         <v>5</v>
@@ -2980,7 +2987,7 @@
       </c>
       <c r="E97" s="1"/>
       <c r="F97" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G97">
         <v>5</v>
@@ -3001,7 +3008,7 @@
       </c>
       <c r="E98" s="1"/>
       <c r="F98" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G98">
         <v>3</v>
@@ -3022,7 +3029,7 @@
       </c>
       <c r="E99" s="1"/>
       <c r="F99" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G99">
         <v>3</v>
@@ -3042,10 +3049,10 @@
         <v>9</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F100" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G100">
         <v>3</v>
@@ -3066,7 +3073,7 @@
       </c>
       <c r="E101" s="1"/>
       <c r="F101" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G101">
         <v>3</v>
@@ -3087,7 +3094,7 @@
       </c>
       <c r="E102" s="1"/>
       <c r="F102" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G102">
         <v>3</v>
@@ -3108,7 +3115,7 @@
       </c>
       <c r="E103" s="1"/>
       <c r="F103" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G103">
         <v>3</v>
@@ -3129,7 +3136,7 @@
       </c>
       <c r="E104" s="1"/>
       <c r="F104" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G104">
         <v>3</v>
@@ -3149,10 +3156,10 @@
         <v>12</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F105" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G105">
         <v>3</v>
@@ -3172,10 +3179,10 @@
         <v>13</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F106" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G106">
         <v>3</v>
@@ -3196,7 +3203,7 @@
       </c>
       <c r="E107" s="1"/>
       <c r="F107" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G107">
         <v>3</v>
@@ -3217,7 +3224,7 @@
       </c>
       <c r="E108" s="1"/>
       <c r="F108" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G108">
         <v>3</v>
@@ -3238,7 +3245,7 @@
       </c>
       <c r="E109" s="1"/>
       <c r="F109" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G109">
         <v>3</v>

</xml_diff>

<commit_message>
Snap Share implementation across TP, PP, SC
</commit_message>
<xml_diff>
--- a/data/drafts.xlsx
+++ b/data/drafts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max/Insync/rmaxsm@umich.edu/Google Drive/FF/TRUFFLE/TRUFFLEdashGIT/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CDAA329-A6FC-6F43-9778-9287A1EF7702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28F3044B-F99B-724E-B3AF-91A083F364FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{9C0D35C5-E0BD-F642-9C22-EDCA1069C401}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{9C0D35C5-E0BD-F642-9C22-EDCA1069C401}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="132">
   <si>
     <t>Season</t>
   </si>
@@ -120,27 +120,18 @@
     <t>Ke'Shawn Vaughn</t>
   </si>
   <si>
-    <t>Henry Ruggs III</t>
-  </si>
-  <si>
     <t>AJ Dillon</t>
   </si>
   <si>
     <t>Justin Jefferson</t>
   </si>
   <si>
-    <t>Michael Pittman Jr</t>
-  </si>
-  <si>
     <t>Antonio Gibson</t>
   </si>
   <si>
     <t>Tee Higgins</t>
   </si>
   <si>
-    <t>Laviska Shenault Jr</t>
-  </si>
-  <si>
     <t>Brandon Aiyuk</t>
   </si>
   <si>
@@ -156,12 +147,6 @@
     <t>KJ Hamler</t>
   </si>
   <si>
-    <t>Lynn Bowden Jr</t>
-  </si>
-  <si>
-    <t>Anthony McFarland Jr</t>
-  </si>
-  <si>
     <t>Van Jefferson</t>
   </si>
   <si>
@@ -240,15 +225,9 @@
     <t>Michael Carter</t>
   </si>
   <si>
-    <t>Amon-Ra St. Brown</t>
-  </si>
-  <si>
     <t>Rashod Bateman</t>
   </si>
   <si>
-    <t>Terrace Marshall Jr</t>
-  </si>
-  <si>
     <t>Chuba Hubbard</t>
   </si>
   <si>
@@ -333,9 +312,6 @@
     <t>Drake London</t>
   </si>
   <si>
-    <t>Kenneth Walker III</t>
-  </si>
-  <si>
     <t>Garrett Wilson</t>
   </si>
   <si>
@@ -387,9 +363,6 @@
     <t>David Bell</t>
   </si>
   <si>
-    <t>John Metchie III</t>
-  </si>
-  <si>
     <t>Sam Howell</t>
   </si>
   <si>
@@ -426,7 +399,37 @@
     <t>Khalil Shakir</t>
   </si>
   <si>
-    <t>Brian Robinson Jr.</t>
+    <t>Extension</t>
+  </si>
+  <si>
+    <t>Brian Robinson</t>
+  </si>
+  <si>
+    <t>John Metchie</t>
+  </si>
+  <si>
+    <t>Kenneth Walker</t>
+  </si>
+  <si>
+    <t>Terrace Marshall</t>
+  </si>
+  <si>
+    <t>Laviska Shenault</t>
+  </si>
+  <si>
+    <t>Anthony McFarland</t>
+  </si>
+  <si>
+    <t>Lynn Bowden</t>
+  </si>
+  <si>
+    <t>Henry Ruggs</t>
+  </si>
+  <si>
+    <t>Michael Pittman</t>
+  </si>
+  <si>
+    <t>Amon-Ra St Brown</t>
   </si>
 </sst>
 </file>
@@ -787,8 +790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{133FC257-8E11-CE40-AF62-7EB48A446FE4}">
   <dimension ref="A1:T109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E109" sqref="E109"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="H110" sqref="H110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -804,10 +807,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="D1" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -817,6 +820,9 @@
       </c>
       <c r="G1" t="s">
         <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
@@ -836,12 +842,14 @@
         <v>17</v>
       </c>
       <c r="F2" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="G2">
         <v>50</v>
       </c>
-      <c r="H2" s="1"/>
+      <c r="H2" s="1">
+        <v>70</v>
+      </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -871,10 +879,13 @@
         <v>18</v>
       </c>
       <c r="F3" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="G3">
         <v>45</v>
+      </c>
+      <c r="H3">
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
@@ -894,10 +905,13 @@
         <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G4">
         <v>40</v>
+      </c>
+      <c r="H4">
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
@@ -917,10 +931,13 @@
         <v>20</v>
       </c>
       <c r="F5" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G5">
         <v>35</v>
+      </c>
+      <c r="H5">
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
@@ -940,10 +957,13 @@
         <v>21</v>
       </c>
       <c r="F6" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="G6">
         <v>30</v>
+      </c>
+      <c r="H6">
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
@@ -963,12 +983,14 @@
         <v>22</v>
       </c>
       <c r="F7" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G7">
         <v>25</v>
       </c>
-      <c r="H7" s="1"/>
+      <c r="H7" s="1">
+        <v>60</v>
+      </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -998,10 +1020,13 @@
         <v>23</v>
       </c>
       <c r="F8" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G8">
         <v>20</v>
+      </c>
+      <c r="H8">
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
@@ -1021,10 +1046,13 @@
         <v>24</v>
       </c>
       <c r="F9" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G9">
         <v>15</v>
+      </c>
+      <c r="H9">
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
@@ -1041,13 +1069,16 @@
         <v>13</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="F10" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G10">
         <v>15</v>
+      </c>
+      <c r="H10">
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
@@ -1067,10 +1098,13 @@
         <v>25</v>
       </c>
       <c r="F11" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G11">
         <v>10</v>
+      </c>
+      <c r="H11">
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
@@ -1090,12 +1124,14 @@
         <v>26</v>
       </c>
       <c r="F12" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G12">
         <v>10</v>
       </c>
-      <c r="H12" s="1"/>
+      <c r="H12" s="1">
+        <v>50</v>
+      </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
@@ -1125,10 +1161,13 @@
         <v>27</v>
       </c>
       <c r="F13" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G13">
         <v>10</v>
+      </c>
+      <c r="H13">
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
@@ -1145,13 +1184,16 @@
         <v>16</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>28</v>
+        <v>129</v>
       </c>
       <c r="F14" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G14">
         <v>5</v>
+      </c>
+      <c r="H14">
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
@@ -1168,13 +1210,16 @@
         <v>15</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F15" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G15">
         <v>5</v>
+      </c>
+      <c r="H15">
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
@@ -1191,16 +1236,19 @@
         <v>14</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F16" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G16">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H16">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2020</v>
       </c>
@@ -1214,16 +1262,19 @@
         <v>13</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>31</v>
+        <v>130</v>
       </c>
       <c r="F17" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G17">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H17">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2020</v>
       </c>
@@ -1237,16 +1288,19 @@
         <v>12</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F18" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G18">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H18">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2020</v>
       </c>
@@ -1260,16 +1314,19 @@
         <v>11</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F19" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G19">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H19">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2020</v>
       </c>
@@ -1283,16 +1340,19 @@
         <v>13</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>34</v>
+        <v>126</v>
       </c>
       <c r="F20" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G20">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H20">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2020</v>
       </c>
@@ -1306,16 +1366,19 @@
         <v>9</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F21" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G21">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H21">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2020</v>
       </c>
@@ -1329,16 +1392,19 @@
         <v>8</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F22" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G22">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H22">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2020</v>
       </c>
@@ -1352,16 +1418,19 @@
         <v>10</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F23" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="G23">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H23">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2020</v>
       </c>
@@ -1375,16 +1444,19 @@
         <v>6</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F24" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G24">
         <v>4</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H24">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2020</v>
       </c>
@@ -1398,16 +1470,19 @@
         <v>5</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F25" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G25">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2020</v>
       </c>
@@ -1421,16 +1496,19 @@
         <v>5</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>40</v>
+        <v>128</v>
       </c>
       <c r="F26" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G26">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H26">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2020</v>
       </c>
@@ -1444,16 +1522,19 @@
         <v>6</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>41</v>
+        <v>127</v>
       </c>
       <c r="F27" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G27">
         <v>3</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H27">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2020</v>
       </c>
@@ -1467,16 +1548,19 @@
         <v>10</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F28" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G28">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H28">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2020</v>
       </c>
@@ -1490,16 +1574,19 @@
         <v>8</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="F29" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G29">
         <v>3</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H29">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2020</v>
       </c>
@@ -1513,16 +1600,19 @@
         <v>9</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F30" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G30">
         <v>3</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H30">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>2020</v>
       </c>
@@ -1536,16 +1626,19 @@
         <v>7</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F31" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="G31">
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2020</v>
       </c>
@@ -1559,13 +1652,16 @@
         <v>11</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F32" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G32">
         <v>3</v>
+      </c>
+      <c r="H32">
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.2">
@@ -1582,13 +1678,16 @@
         <v>12</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F33" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="G33">
         <v>3</v>
+      </c>
+      <c r="H33">
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.2">
@@ -1605,13 +1704,16 @@
         <v>10</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F34" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="G34">
         <v>3</v>
+      </c>
+      <c r="H34">
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.2">
@@ -1628,13 +1730,16 @@
         <v>14</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F35" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G35">
         <v>3</v>
+      </c>
+      <c r="H35">
+        <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.2">
@@ -1651,13 +1756,16 @@
         <v>15</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F36" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G36">
         <v>3</v>
+      </c>
+      <c r="H36">
+        <v>30</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.2">
@@ -1674,13 +1782,16 @@
         <v>16</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F37" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G37">
         <v>3</v>
+      </c>
+      <c r="H37">
+        <v>30</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.2">
@@ -1697,15 +1808,17 @@
         <v>14</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="F38" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="G38">
         <v>50</v>
       </c>
-      <c r="H38" s="1"/>
+      <c r="H38" s="1">
+        <v>70</v>
+      </c>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
@@ -1732,13 +1845,16 @@
         <v>6</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F39" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="G39">
         <v>45</v>
+      </c>
+      <c r="H39">
+        <v>70</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.2">
@@ -1755,13 +1871,16 @@
         <v>13</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F40" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G40">
         <v>40</v>
+      </c>
+      <c r="H40">
+        <v>60</v>
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.2">
@@ -1778,13 +1897,16 @@
         <v>9</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F41" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="G41">
         <v>35</v>
+      </c>
+      <c r="H41">
+        <v>30</v>
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.2">
@@ -1801,15 +1923,17 @@
         <v>5</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F42" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="G42">
         <v>30</v>
       </c>
-      <c r="H42" s="1"/>
+      <c r="H42" s="1">
+        <v>70</v>
+      </c>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
@@ -1836,13 +1960,16 @@
         <v>11</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F43" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G43">
         <v>25</v>
+      </c>
+      <c r="H43">
+        <v>70</v>
       </c>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.2">
@@ -1859,13 +1986,16 @@
         <v>13</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F44" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="G44">
         <v>20</v>
+      </c>
+      <c r="H44">
+        <v>60</v>
       </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.2">
@@ -1882,13 +2012,16 @@
         <v>12</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F45" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G45">
         <v>15</v>
+      </c>
+      <c r="H45">
+        <v>50</v>
       </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.2">
@@ -1905,13 +2038,16 @@
         <v>15</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F46" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="G46">
         <v>15</v>
+      </c>
+      <c r="H46">
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.2">
@@ -1928,13 +2064,16 @@
         <v>10</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F47" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G47">
         <v>10</v>
+      </c>
+      <c r="H47">
+        <v>50</v>
       </c>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.2">
@@ -1951,13 +2090,16 @@
         <v>10</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F48" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G48">
         <v>10</v>
+      </c>
+      <c r="H48">
+        <v>60</v>
       </c>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.2">
@@ -1974,13 +2116,16 @@
         <v>8</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F49" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G49">
         <v>10</v>
+      </c>
+      <c r="H49">
+        <v>50</v>
       </c>
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.2">
@@ -1997,13 +2142,16 @@
         <v>9</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F50" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G50">
         <v>5</v>
+      </c>
+      <c r="H50">
+        <v>50</v>
       </c>
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.2">
@@ -2020,13 +2168,16 @@
         <v>7</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F51" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G51">
         <v>5</v>
+      </c>
+      <c r="H51">
+        <v>50</v>
       </c>
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.2">
@@ -2043,13 +2194,16 @@
         <v>7</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F52" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G52">
         <v>5</v>
+      </c>
+      <c r="H52">
+        <v>40</v>
       </c>
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.2">
@@ -2066,13 +2220,16 @@
         <v>16</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="F53" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G53">
         <v>5</v>
+      </c>
+      <c r="H53">
+        <v>50</v>
       </c>
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.2">
@@ -2089,13 +2246,16 @@
         <v>12</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>68</v>
+        <v>131</v>
       </c>
       <c r="F54" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G54">
         <v>5</v>
+      </c>
+      <c r="H54">
+        <v>40</v>
       </c>
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.2">
@@ -2112,13 +2272,16 @@
         <v>11</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F55" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G55">
         <v>5</v>
+      </c>
+      <c r="H55">
+        <v>40</v>
       </c>
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.2">
@@ -2135,13 +2298,16 @@
         <v>11</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>70</v>
+        <v>125</v>
       </c>
       <c r="F56" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G56">
         <v>4</v>
+      </c>
+      <c r="H56">
+        <v>40</v>
       </c>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.2">
@@ -2158,13 +2324,16 @@
         <v>5</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="F57" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G57">
         <v>4</v>
+      </c>
+      <c r="H57">
+        <v>50</v>
       </c>
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.2">
@@ -2181,13 +2350,16 @@
         <v>9</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="F58" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G58">
         <v>4</v>
+      </c>
+      <c r="H58">
+        <v>40</v>
       </c>
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.2">
@@ -2204,13 +2376,16 @@
         <v>16</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="F59" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G59">
         <v>4</v>
+      </c>
+      <c r="H59">
+        <v>40</v>
       </c>
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.2">
@@ -2227,13 +2402,16 @@
         <v>6</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="F60" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G60">
         <v>4</v>
+      </c>
+      <c r="H60">
+        <v>40</v>
       </c>
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.2">
@@ -2250,13 +2428,16 @@
         <v>14</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="F61" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="G61">
         <v>4</v>
+      </c>
+      <c r="H61">
+        <v>40</v>
       </c>
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.2">
@@ -2273,13 +2454,16 @@
         <v>14</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="F62" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="G62">
         <v>3</v>
+      </c>
+      <c r="H62">
+        <v>5</v>
       </c>
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.2">
@@ -2296,13 +2480,16 @@
         <v>6</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="F63" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G63">
         <v>3</v>
+      </c>
+      <c r="H63">
+        <v>30</v>
       </c>
       <c r="I63" s="1"/>
       <c r="J63" s="1"/>
@@ -2331,16 +2518,19 @@
         <v>7</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="F64" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="G64">
         <v>3</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H64">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>2021</v>
       </c>
@@ -2354,16 +2544,19 @@
         <v>9</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="F65" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="G65">
         <v>3</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H65">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>2021</v>
       </c>
@@ -2377,16 +2570,19 @@
         <v>5</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F66" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G66">
         <v>3</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H66">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>2021</v>
       </c>
@@ -2400,16 +2596,19 @@
         <v>13</v>
       </c>
       <c r="E67" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F67" t="s">
         <v>81</v>
       </c>
-      <c r="F67" t="s">
-        <v>88</v>
-      </c>
       <c r="G67">
         <v>3</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H67">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>2021</v>
       </c>
@@ -2423,16 +2622,19 @@
         <v>14</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F68" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G68">
         <v>3</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H68">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>2021</v>
       </c>
@@ -2446,16 +2648,19 @@
         <v>12</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="F69" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G69">
         <v>3</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H69">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>2021</v>
       </c>
@@ -2469,16 +2674,19 @@
         <v>16</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="F70" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G70">
         <v>3</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H70">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>2021</v>
       </c>
@@ -2492,16 +2700,19 @@
         <v>11</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="F71" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G71">
         <v>3</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H71">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>2021</v>
       </c>
@@ -2515,16 +2726,19 @@
         <v>10</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="F72" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G72">
         <v>3</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H72">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>2021</v>
       </c>
@@ -2538,16 +2752,19 @@
         <v>8</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F73" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G73">
         <v>3</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H73">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>2022</v>
       </c>
@@ -2561,16 +2778,19 @@
         <v>12</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="F74" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G74">
         <v>50</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H74">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>2022</v>
       </c>
@@ -2584,16 +2804,19 @@
         <v>6</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="F75" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G75">
         <v>45</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H75">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>2022</v>
       </c>
@@ -2607,16 +2830,19 @@
         <v>16</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="F76" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G76">
         <v>40</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H76">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>2022</v>
       </c>
@@ -2630,16 +2856,19 @@
         <v>7</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="F77" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G77">
         <v>35</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H77">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>2022</v>
       </c>
@@ -2653,16 +2882,19 @@
         <v>15</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>99</v>
+        <v>124</v>
       </c>
       <c r="F78" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G78">
         <v>30</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H78">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>2022</v>
       </c>
@@ -2676,16 +2908,19 @@
         <v>5</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="F79" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G79">
         <v>25</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H79">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>2022</v>
       </c>
@@ -2699,16 +2934,19 @@
         <v>14</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="F80" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G80">
         <v>20</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H80">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>2022</v>
       </c>
@@ -2722,16 +2960,19 @@
         <v>16</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="F81" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G81">
         <v>15</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H81">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>2022</v>
       </c>
@@ -2745,16 +2986,19 @@
         <v>8</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="F82" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G82">
         <v>15</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H82">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>2022</v>
       </c>
@@ -2768,16 +3012,19 @@
         <v>7</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="F83" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="G83">
         <v>10</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H83">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>2022</v>
       </c>
@@ -2791,16 +3038,19 @@
         <v>15</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="F84" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G84">
         <v>10</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H84">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>2022</v>
       </c>
@@ -2814,16 +3064,19 @@
         <v>11</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="F85" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G85">
         <v>10</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H85">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>2022</v>
       </c>
@@ -2837,16 +3090,19 @@
         <v>11</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="F86" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="G86">
         <v>5</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H86">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>2022</v>
       </c>
@@ -2860,16 +3116,19 @@
         <v>5</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="F87" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G87">
         <v>5</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H87">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>2022</v>
       </c>
@@ -2883,16 +3142,19 @@
         <v>7</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="F88" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G88">
         <v>5</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H88">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>2022</v>
       </c>
@@ -2906,16 +3168,19 @@
         <v>8</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="F89" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G89">
         <v>5</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H89">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>2022</v>
       </c>
@@ -2929,16 +3194,19 @@
         <v>12</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="F90" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="G90">
         <v>5</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H90">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>2022</v>
       </c>
@@ -2952,16 +3220,19 @@
         <v>14</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="F91" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G91">
         <v>5</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H91">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>2022</v>
       </c>
@@ -2975,16 +3246,19 @@
         <v>5</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="F92" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="G92">
         <v>5</v>
       </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H92">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>2022</v>
       </c>
@@ -2998,16 +3272,19 @@
         <v>9</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="F93" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G93">
         <v>5</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H93">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>2022</v>
       </c>
@@ -3021,16 +3298,19 @@
         <v>9</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="F94" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G94">
         <v>5</v>
       </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H94">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>2022</v>
       </c>
@@ -3044,16 +3324,19 @@
         <v>16</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="F95" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G95">
         <v>5</v>
       </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H95">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>2022</v>
       </c>
@@ -3067,16 +3350,19 @@
         <v>6</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="F96" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G96">
         <v>5</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H96">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>2022</v>
       </c>
@@ -3090,16 +3376,19 @@
         <v>15</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="F97" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G97">
         <v>5</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H97">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>2022</v>
       </c>
@@ -3113,16 +3402,19 @@
         <v>15</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="F98" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="G98">
         <v>3</v>
       </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H98">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>2022</v>
       </c>
@@ -3136,16 +3428,19 @@
         <v>6</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="F99" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G99">
         <v>3</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H99">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>2022</v>
       </c>
@@ -3159,16 +3454,19 @@
         <v>9</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="F100" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="G100">
         <v>3</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H100">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>2022</v>
       </c>
@@ -3182,16 +3480,19 @@
         <v>7</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="F101" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G101">
         <v>3</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H101">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>2022</v>
       </c>
@@ -3205,16 +3506,19 @@
         <v>12</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="F102" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G102">
         <v>3</v>
       </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H102">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>2022</v>
       </c>
@@ -3228,16 +3532,19 @@
         <v>5</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="F103" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="G103">
         <v>3</v>
       </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H103">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>2022</v>
       </c>
@@ -3251,16 +3558,19 @@
         <v>14</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="F104" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G104">
         <v>3</v>
       </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H104">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>2022</v>
       </c>
@@ -3274,16 +3584,19 @@
         <v>12</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="F105" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G105">
         <v>3</v>
       </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H105">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>2022</v>
       </c>
@@ -3297,16 +3610,19 @@
         <v>13</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="F106" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="G106">
         <v>3</v>
       </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H106">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>2022</v>
       </c>
@@ -3320,16 +3636,19 @@
         <v>10</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="F107" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="G107">
         <v>3</v>
       </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H107">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>2022</v>
       </c>
@@ -3343,16 +3662,19 @@
         <v>13</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="F108" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G108">
         <v>3</v>
       </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H108">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>2022</v>
       </c>
@@ -3366,13 +3688,16 @@
         <v>11</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="F109" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="G109">
         <v>3</v>
+      </c>
+      <c r="H109">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>